<commit_message>
Added policyForm, Year built, older Reneovated Home
</commit_message>
<xml_diff>
--- a/THS_TestData.xlsx
+++ b/THS_TestData.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>GroupID</t>
   </si>
@@ -79,22 +79,43 @@
     <t>FireHyderate</t>
   </si>
   <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Tuscaloosa</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>4410 Woodland Hills Dr</t>
+    <t>YearBuilt</t>
+  </si>
+  <si>
+    <t>ReneovatedHome</t>
+  </si>
+  <si>
+    <t>195 Painted Desert Ln</t>
+  </si>
+  <si>
+    <t>Buda</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>PolicyForm</t>
+  </si>
+  <si>
+    <t>DP-3</t>
+  </si>
+  <si>
+    <t>Seasonal</t>
+  </si>
+  <si>
+    <t>312 Saddle Wood Dr</t>
+  </si>
+  <si>
+    <t>Canton</t>
+  </si>
+  <si>
+    <t>WI</t>
   </si>
 </sst>
 </file>
@@ -133,12 +154,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G2" sqref="A1:M2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,10 +462,13 @@
     <col min="11" max="11" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,7 +494,7 @@
         <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>15</v>
@@ -483,8 +508,17 @@
       <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -504,25 +538,34 @@
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="J2" s="2">
-        <v>35405</v>
+        <v>30114</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="N2" s="2">
+        <v>2000</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -533,14 +576,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2">
+        <v>78610</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated DataProvider! and discription for each test case
</commit_message>
<xml_diff>
--- a/THS_TestData.xlsx
+++ b/THS_TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>GroupID</t>
   </si>
@@ -103,19 +103,103 @@
     <t>PolicyForm</t>
   </si>
   <si>
-    <t>DP-3</t>
-  </si>
-  <si>
-    <t>Seasonal</t>
-  </si>
-  <si>
-    <t>312 Saddle Wood Dr</t>
-  </si>
-  <si>
-    <t>Canton</t>
-  </si>
-  <si>
-    <t>WI</t>
+    <t>2252 PARTRIDGE LN</t>
+  </si>
+  <si>
+    <t>HOOVER</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>12100 midpines DR</t>
+  </si>
+  <si>
+    <t>Cincinnati</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>116 SW Wind Ridge Dr</t>
+  </si>
+  <si>
+    <t>Lees Summit</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">522 Walnut St </t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>215 Leith Way</t>
+  </si>
+  <si>
+    <t>Cary</t>
+  </si>
+  <si>
+    <t>6734 Jordan Run Rd</t>
+  </si>
+  <si>
+    <t>Chattanooga</t>
+  </si>
+  <si>
+    <t>DP1</t>
+  </si>
+  <si>
+    <t>DP3</t>
+  </si>
+  <si>
+    <t>HO3</t>
+  </si>
+  <si>
+    <t>HO6</t>
+  </si>
+  <si>
+    <t>MH</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>406 Lockshire Rd</t>
+  </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>106 Hunter Trl</t>
+  </si>
+  <si>
+    <t>Florence</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>DP-1</t>
+  </si>
+  <si>
+    <t>LA</t>
   </si>
 </sst>
 </file>
@@ -154,13 +238,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J6" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,11 +546,11 @@
     <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="1"/>
     <col min="11" max="11" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="12" max="12" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -537,26 +627,26 @@
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="2">
-        <v>30114</v>
+      <c r="G2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="5">
+        <v>29212</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="N2" s="2">
         <v>2000</v>
@@ -564,8 +654,8 @@
       <c r="O2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>27</v>
+      <c r="P2" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -576,18 +666,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D2"/>
+  <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="A9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -597,8 +689,135 @@
       <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>78610</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="5">
+        <v>45241</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="5">
+        <v>64081</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="5">
+        <v>47250</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="5">
+        <v>60013</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="5">
+        <v>37412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4">
+        <v>35226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="5">
+        <v>29212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="5">
+        <v>39073</v>
       </c>
     </row>
   </sheetData>

</xml_diff>